<commit_message>
solving algorithmic tasks from yandex academy
</commit_message>
<xml_diff>
--- a/горячие клавиши в VS Code.xlsx
+++ b/горячие клавиши в VS Code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fess\Google Диск\project\обучение\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D0C452-F7F4-4C83-8683-04B4289A1C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F4A64A-F65B-414B-BF88-31A0F4355804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>https://www.nikomedvedev.ru/other/vscodeshortcuts/hotkeys.html</t>
+  </si>
+  <si>
+    <t>Ctrl + P</t>
+  </si>
+  <si>
+    <t>Быстрый переход к файлу</t>
+  </si>
+  <si>
+    <t>Ctrl + G</t>
+  </si>
+  <si>
+    <t>Перейти к строке</t>
+  </si>
+  <si>
+    <t>alt+shift+down</t>
+  </si>
+  <si>
+    <t>Копировать текущую строку вниз</t>
+  </si>
+  <si>
+    <t>Alt + Enter</t>
+  </si>
+  <si>
+    <t>Выделить все вхождения при поиске</t>
+  </si>
+  <si>
+    <t>ctrl+tab</t>
+  </si>
+  <si>
+    <t>слудущая вкладка</t>
+  </si>
+  <si>
+    <t>Alt + Z</t>
+  </si>
+  <si>
+    <t>Вкл. / выкл. перенос текста</t>
+  </si>
+  <si>
+    <t>Alt + Shift + →</t>
+  </si>
+  <si>
+    <t>Расширить выделение</t>
+  </si>
+  <si>
+    <t>можно сразу всю функцию выбрать</t>
+  </si>
+  <si>
+    <t>описание</t>
+  </si>
+  <si>
+    <t>комментарии</t>
+  </si>
+  <si>
+    <t>Добавить курсор</t>
+  </si>
+  <si>
+    <t>Alt + Click</t>
+  </si>
+  <si>
+    <t>смешная штука</t>
+  </si>
+  <si>
+    <t>Alt + Shift + ↑</t>
+  </si>
+  <si>
+    <t>Добавить курсор выше</t>
+  </si>
+  <si>
+    <t>ниже так же</t>
+  </si>
+  <si>
+    <t>Переместить строку вниз</t>
+  </si>
+  <si>
+    <t>Alt + вниз</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + L</t>
+  </si>
+  <si>
+    <t>Выбрать все вхождения</t>
+  </si>
+  <si>
+    <t>выделяются все такие же элементы, можно редактировать</t>
+  </si>
+  <si>
+    <t>Ctrl + F2</t>
+  </si>
+  <si>
+    <t>Выделить все вхождения текущего слова</t>
+  </si>
+  <si>
+    <t>Ctrl + Enter</t>
+  </si>
+  <si>
+    <t>Вставить пустую строку ниже</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + Enter</t>
+  </si>
+  <si>
+    <t>Вставить пустую строку выше</t>
+  </si>
+  <si>
+    <t>Ctrl + ]</t>
+  </si>
+  <si>
+    <t>Увеличить табуляцию для строки</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift+J</t>
+  </si>
+  <si>
+    <t>свернуть(fold) все вложенные участки</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift+H</t>
+  </si>
+  <si>
+    <t>развернуть(fold) все вложенные участки</t>
+  </si>
+  <si>
+    <t>есть тема для разных уровней вложенности!</t>
+  </si>
+  <si>
+    <t>Ctrl+Alt+/</t>
+  </si>
+  <si>
+    <t>свернуть(fold) первый уровень</t>
+  </si>
+  <si>
+    <t>режим zen</t>
+  </si>
+  <si>
+    <t>открывает чисто нужный код на весь экран</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +177,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -59,14 +214,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,23 +583,932 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCellId="1" sqref="A4 A1"/>
+      <selection activeCell="C20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="77.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{71DE7317-8887-489D-9FA2-A1DD837B7417}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>